<commit_message>
[ADD]Add menu for notifications
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyongle/Documents/work/devops-service/src/main/resources/script/front/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3442D85E-C80E-7346-8B29-62A6FA4485B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7373747F-B324-2D40-A3C7-26BA328B10AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1840" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="404">
   <si>
     <t>IAM_PERMISSION</t>
   </si>
@@ -1229,6 +1229,74 @@
   </si>
   <si>
     <t>database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>choerodon.code.prosetting.element-settings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>通知设置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>choerodon.code.prosetting.devops-notifications</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notifications</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>choerodon.route.prosetting.element-settings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>choerodon.route.prosetting.devops-notifications</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu_item</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>notifications</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/devops/notifications</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>通知设置路由</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.listByOptions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.create</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.update</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.queryById</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>devops-service.devops-notification.delete</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1236,7 +1304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
@@ -1254,6 +1322,11 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1276,10 +1349,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1582,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A7:AMK37"/>
+  <dimension ref="A7:AMK38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="157" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B5" zoomScale="157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -2482,32 +2556,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="6:14">
-      <c r="F37" t="s">
+    <row r="37" spans="6:14" s="1" customFormat="1">
+      <c r="F37" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:14">
+      <c r="F38" t="s">
         <v>102</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>103</v>
       </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" t="s">
         <v>104</v>
       </c>
-      <c r="K37" t="s">
+      <c r="K38" t="s">
         <v>16</v>
       </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
         <v>1</v>
       </c>
-      <c r="N37">
+      <c r="N38">
         <v>0</v>
       </c>
     </row>
@@ -2524,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A7:AMK46"/>
+  <dimension ref="A7:AMK47"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" zoomScale="166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView topLeftCell="F22" zoomScale="166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -3716,7 +3819,7 @@
     </row>
     <row r="44" spans="6:15">
       <c r="F44" t="s">
-        <v>219</v>
+        <v>387</v>
       </c>
       <c r="G44" t="s">
         <v>220</v>
@@ -3725,7 +3828,7 @@
         <v>221</v>
       </c>
       <c r="I44" t="s">
-        <v>99</v>
+        <v>391</v>
       </c>
       <c r="J44" t="s">
         <v>13</v>
@@ -3746,64 +3849,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="6:15">
-      <c r="F45" t="s">
-        <v>222</v>
-      </c>
-      <c r="G45" t="s">
-        <v>223</v>
-      </c>
-      <c r="H45" t="s">
-        <v>224</v>
-      </c>
-      <c r="J45" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" t="s">
-        <v>131</v>
-      </c>
-      <c r="L45" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" t="s">
-        <v>117</v>
-      </c>
-      <c r="N45" t="s">
-        <v>369</v>
-      </c>
-      <c r="O45">
-        <v>99</v>
+    <row r="45" spans="6:15" s="1" customFormat="1">
+      <c r="F45" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="O45" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="6:15">
       <c r="F46" t="s">
+        <v>222</v>
+      </c>
+      <c r="G46" t="s">
+        <v>223</v>
+      </c>
+      <c r="H46" t="s">
+        <v>224</v>
+      </c>
+      <c r="J46" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" t="s">
+        <v>131</v>
+      </c>
+      <c r="L46" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" t="s">
+        <v>117</v>
+      </c>
+      <c r="N46" t="s">
+        <v>369</v>
+      </c>
+      <c r="O46">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="6:15">
+      <c r="F47" t="s">
         <v>225</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>226</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" t="s">
         <v>227</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>102</v>
       </c>
-      <c r="J46" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
         <v>222</v>
       </c>
-      <c r="L46" t="s">
-        <v>25</v>
-      </c>
-      <c r="M46" t="s">
+      <c r="L47" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" t="s">
         <v>121</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N47" t="s">
         <v>371</v>
       </c>
-      <c r="O46">
+      <c r="O47">
         <v>2</v>
       </c>
     </row>
@@ -3820,10 +3955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A7:AMK155"/>
+  <dimension ref="A7:AMK161"/>
   <sheetViews>
-    <sheetView topLeftCell="C103" zoomScale="172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="D120" zoomScale="172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -4938,52 +5073,52 @@
         <v>331</v>
       </c>
     </row>
-    <row r="144" spans="6:7">
-      <c r="F144" t="s">
-        <v>225</v>
-      </c>
-      <c r="G144" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="145" spans="6:7">
-      <c r="F145" t="s">
-        <v>225</v>
-      </c>
-      <c r="G145" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="146" spans="6:7">
-      <c r="F146" t="s">
-        <v>225</v>
-      </c>
-      <c r="G146" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="147" spans="6:7">
-      <c r="F147" t="s">
-        <v>225</v>
-      </c>
-      <c r="G147" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="148" spans="6:7">
-      <c r="F148" t="s">
-        <v>225</v>
-      </c>
-      <c r="G148" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="149" spans="6:7">
-      <c r="F149" t="s">
-        <v>225</v>
-      </c>
-      <c r="G149" t="s">
-        <v>279</v>
+    <row r="144" spans="6:7" s="1" customFormat="1">
+      <c r="F144" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="6:7" s="1" customFormat="1">
+      <c r="F145" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="146" spans="6:7" s="1" customFormat="1">
+      <c r="F146" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="147" spans="6:7" s="1" customFormat="1">
+      <c r="F147" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="148" spans="6:7" s="1" customFormat="1">
+      <c r="F148" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="149" spans="6:7" s="1" customFormat="1">
+      <c r="F149" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="6:7">
@@ -4991,7 +5126,7 @@
         <v>225</v>
       </c>
       <c r="G150" t="s">
-        <v>336</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" spans="6:7">
@@ -4999,7 +5134,7 @@
         <v>225</v>
       </c>
       <c r="G151" t="s">
-        <v>253</v>
+        <v>332</v>
       </c>
     </row>
     <row r="152" spans="6:7">
@@ -5007,7 +5142,7 @@
         <v>225</v>
       </c>
       <c r="G152" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="153" spans="6:7">
@@ -5015,7 +5150,7 @@
         <v>225</v>
       </c>
       <c r="G153" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="154" spans="6:7">
@@ -5023,7 +5158,7 @@
         <v>225</v>
       </c>
       <c r="G154" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="155" spans="6:7">
@@ -5031,6 +5166,54 @@
         <v>225</v>
       </c>
       <c r="G155" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="156" spans="6:7">
+      <c r="F156" t="s">
+        <v>225</v>
+      </c>
+      <c r="G156" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="157" spans="6:7">
+      <c r="F157" t="s">
+        <v>225</v>
+      </c>
+      <c r="G157" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="158" spans="6:7">
+      <c r="F158" t="s">
+        <v>225</v>
+      </c>
+      <c r="G158" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="159" spans="6:7">
+      <c r="F159" t="s">
+        <v>225</v>
+      </c>
+      <c r="G159" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="160" spans="6:7">
+      <c r="F160" t="s">
+        <v>225</v>
+      </c>
+      <c r="G160" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="161" spans="6:7">
+      <c r="F161" t="s">
+        <v>225</v>
+      </c>
+      <c r="G161" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP]Set the version to 0.17
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyongle/Documents/work/devops-service/src/main/resources/script/front/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA35BA5-3E13-4346-AF1C-DC14A8EBA835}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9347" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -1209,14 +1215,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
@@ -1230,355 +1230,24 @@
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1586,312 +1255,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2176,37 +1559,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D7:N38"/>
   <sheetViews>
     <sheetView topLeftCell="F13" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6018518518519" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="11.6018518518519" customWidth="1"/>
-    <col min="6" max="6" width="65.7962962962963" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="6" max="6" width="65.796875" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="28.7962962962963" customWidth="1"/>
+    <col min="10" max="10" width="28.796875" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="29.2037037037037" customWidth="1"/>
-    <col min="14" max="14" width="19.3981481481481" customWidth="1"/>
+    <col min="13" max="13" width="29.19921875" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="1025" width="11.6018518518519" customWidth="1"/>
+    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" ht="12.75" customHeight="1" spans="4:14">
+    <row r="7" spans="4:14" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2241,7 +1624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1" spans="6:14">
+    <row r="8" spans="4:14" ht="12.75" customHeight="1">
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="6:14">
+    <row r="9" spans="4:14">
       <c r="F9" t="s">
         <v>17</v>
       </c>
@@ -2299,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="6:14">
+    <row r="10" spans="4:14">
       <c r="F10" t="s">
         <v>20</v>
       </c>
@@ -2328,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="6:14">
+    <row r="11" spans="4:14">
       <c r="F11" t="s">
         <v>23</v>
       </c>
@@ -2357,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="6:14">
+    <row r="12" spans="4:14">
       <c r="F12" t="s">
         <v>27</v>
       </c>
@@ -2386,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="6:14">
+    <row r="13" spans="4:14">
       <c r="F13" t="s">
         <v>30</v>
       </c>
@@ -2415,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="6:14">
+    <row r="14" spans="4:14">
       <c r="F14" t="s">
         <v>33</v>
       </c>
@@ -2444,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="6:14">
+    <row r="15" spans="4:14">
       <c r="F15" t="s">
         <v>36</v>
       </c>
@@ -2473,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="6:14">
+    <row r="16" spans="4:14">
       <c r="F16" t="s">
         <v>39</v>
       </c>
@@ -3082,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="13.2" spans="6:14">
+    <row r="37" spans="6:14">
       <c r="F37" t="s">
         <v>102</v>
       </c>
@@ -3141,8 +2524,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -3151,33 +2535,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D7:O47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6018518518519" customWidth="1"/>
-    <col min="4" max="4" width="15.2037037037037" customWidth="1"/>
-    <col min="5" max="5" width="11.6018518518519" customWidth="1"/>
-    <col min="6" max="6" width="56.2037037037037" customWidth="1"/>
-    <col min="7" max="7" width="18.2037037037037" customWidth="1"/>
-    <col min="8" max="8" width="27.7962962962963" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="6" max="6" width="56.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.19921875" customWidth="1"/>
+    <col min="8" max="8" width="27.796875" customWidth="1"/>
     <col min="9" max="9" width="66" customWidth="1"/>
-    <col min="10" max="10" width="22.6018518518519" customWidth="1"/>
-    <col min="11" max="11" width="47.6018518518519" customWidth="1"/>
-    <col min="12" max="12" width="25.7962962962963" customWidth="1"/>
-    <col min="13" max="13" width="37.7962962962963" customWidth="1"/>
+    <col min="10" max="10" width="22.59765625" customWidth="1"/>
+    <col min="11" max="11" width="47.59765625" customWidth="1"/>
+    <col min="12" max="12" width="25.796875" customWidth="1"/>
+    <col min="13" max="13" width="37.796875" customWidth="1"/>
     <col min="14" max="14" width="27" customWidth="1"/>
-    <col min="15" max="15" width="9.7962962962963" customWidth="1"/>
-    <col min="16" max="1025" width="11.6018518518519" customWidth="1"/>
+    <col min="15" max="15" width="9.796875" customWidth="1"/>
+    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" ht="12.75" customHeight="1" spans="4:15">
+    <row r="7" spans="4:15" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>108</v>
       </c>
@@ -3215,7 +2598,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1" spans="6:15">
+    <row r="8" spans="4:15" ht="12.75" customHeight="1">
       <c r="F8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3244,7 +2627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="6:15">
+    <row r="9" spans="4:15">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -3276,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="6:15">
+    <row r="10" spans="4:15">
       <c r="F10" t="s">
         <v>126</v>
       </c>
@@ -3308,7 +2691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="6:15">
+    <row r="11" spans="4:15">
       <c r="F11" t="s">
         <v>130</v>
       </c>
@@ -3340,7 +2723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="6:15">
+    <row r="12" spans="4:15">
       <c r="F12" t="s">
         <v>134</v>
       </c>
@@ -3369,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="6:15">
+    <row r="13" spans="4:15">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -3401,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="6:15">
+    <row r="14" spans="4:15">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -3433,7 +2816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="6:15">
+    <row r="15" spans="4:15">
       <c r="F15" t="s">
         <v>147</v>
       </c>
@@ -3465,7 +2848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="6:15">
+    <row r="16" spans="4:15">
       <c r="F16" t="s">
         <v>151</v>
       </c>
@@ -3523,7 +2906,7 @@
         <v>158</v>
       </c>
       <c r="O17">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="6:15">
@@ -3776,7 +3159,7 @@
         <v>190</v>
       </c>
       <c r="O25">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="6:15">
@@ -3939,7 +3322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" customFormat="1" spans="6:15">
+    <row r="31" spans="6:15">
       <c r="F31" t="s">
         <v>211</v>
       </c>
@@ -3968,7 +3351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" customFormat="1" spans="6:15">
+    <row r="32" spans="6:15">
       <c r="F32" t="s">
         <v>215</v>
       </c>
@@ -3997,7 +3380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="1" spans="6:15">
+    <row r="33" spans="6:15">
       <c r="F33" t="s">
         <v>219</v>
       </c>
@@ -4375,7 +3758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" customFormat="1" spans="6:15">
+    <row r="45" spans="6:15">
       <c r="F45" t="s">
         <v>266</v>
       </c>
@@ -4469,8 +3852,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -4479,25 +3863,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D133" workbookViewId="0">
-      <selection activeCell="F152" sqref="D7:G161"/>
+    <sheetView topLeftCell="D133" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6018518518519" customWidth="1"/>
-    <col min="4" max="4" width="23.7962962962963" customWidth="1"/>
-    <col min="5" max="5" width="11.6018518518519" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="23.796875" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
     <col min="6" max="6" width="82" customWidth="1"/>
-    <col min="7" max="7" width="85.2037037037037" customWidth="1"/>
-    <col min="8" max="1025" width="11.6018518518519" customWidth="1"/>
+    <col min="7" max="7" width="85.19921875" customWidth="1"/>
+    <col min="8" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" ht="12.75" customHeight="1" spans="4:7">
+    <row r="7" spans="4:7" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>278</v>
       </c>
@@ -4511,7 +3894,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1" spans="6:7">
+    <row r="8" spans="4:7" ht="12.75" customHeight="1">
       <c r="F8" t="s">
         <v>121</v>
       </c>
@@ -4519,7 +3902,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="6:7">
+    <row r="9" spans="4:7">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -4527,7 +3910,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="6:7">
+    <row r="10" spans="4:7">
       <c r="F10" t="s">
         <v>121</v>
       </c>
@@ -4535,7 +3918,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="6:7">
+    <row r="11" spans="4:7">
       <c r="F11" t="s">
         <v>126</v>
       </c>
@@ -4543,7 +3926,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="6:7">
+    <row r="12" spans="4:7">
       <c r="F12" t="s">
         <v>130</v>
       </c>
@@ -4551,7 +3934,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="6:7">
+    <row r="13" spans="4:7">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -4559,7 +3942,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="6:7">
+    <row r="14" spans="4:7">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -4567,7 +3950,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="6:7">
+    <row r="15" spans="4:7">
       <c r="F15" t="s">
         <v>143</v>
       </c>
@@ -4575,7 +3958,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="6:7">
+    <row r="16" spans="4:7">
       <c r="F16" t="s">
         <v>147</v>
       </c>
@@ -5599,7 +4982,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="144" customFormat="1" spans="6:7">
+    <row r="144" spans="6:7">
       <c r="F144" t="s">
         <v>266</v>
       </c>
@@ -5607,7 +4990,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="145" customFormat="1" spans="6:7">
+    <row r="145" spans="6:7">
       <c r="F145" t="s">
         <v>266</v>
       </c>
@@ -5615,7 +4998,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="146" customFormat="1" spans="6:7">
+    <row r="146" spans="6:7">
       <c r="F146" t="s">
         <v>266</v>
       </c>
@@ -5623,7 +5006,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="147" customFormat="1" spans="6:7">
+    <row r="147" spans="6:7">
       <c r="F147" t="s">
         <v>266</v>
       </c>
@@ -5631,7 +5014,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="148" customFormat="1" spans="6:7">
+    <row r="148" spans="6:7">
       <c r="F148" t="s">
         <v>266</v>
       </c>
@@ -5639,7 +5022,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="149" customFormat="1" spans="6:7">
+    <row r="149" spans="6:7">
       <c r="F149" t="s">
         <v>266</v>
       </c>
@@ -5744,8 +5127,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[ADD]Overwrite the deployment configuration in instance
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyongle/Documents/work/devops-service/src/main/resources/script/front/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA35BA5-3E13-4346-AF1C-DC14A8EBA835}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19935" windowHeight="7785" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -633,6 +627,18 @@
     <t>Operation-monitoring</t>
   </si>
   <si>
+    <t>choerodon.code.deployment-pipeline.deployment-config</t>
+  </si>
+  <si>
+    <t>部署配置</t>
+  </si>
+  <si>
+    <t>Deployment Config</t>
+  </si>
+  <si>
+    <t>cloud_done</t>
+  </si>
+  <si>
     <t>choerodon.code.deployment-pipeline.application-deployment</t>
   </si>
   <si>
@@ -784,18 +790,6 @@
   </si>
   <si>
     <t>format_list_bulleted</t>
-  </si>
-  <si>
-    <t>choerodon.code.deployment-pipeline.deployment-config</t>
-  </si>
-  <si>
-    <t>部署配置</t>
-  </si>
-  <si>
-    <t>Deployment Config</t>
-  </si>
-  <si>
-    <t>cloud_done</t>
   </si>
   <si>
     <t>choerodon.code.prosetting</t>
@@ -1215,8 +1209,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
@@ -1230,24 +1230,355 @@
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1255,26 +1586,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1559,37 +2176,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="D7:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="F13" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="11.59765625" customWidth="1"/>
+    <col min="1" max="3" width="11.6" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" customWidth="1"/>
-    <col min="6" max="6" width="65.796875" customWidth="1"/>
+    <col min="5" max="5" width="11.6" customWidth="1"/>
+    <col min="6" max="6" width="65.8" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="28.796875" customWidth="1"/>
+    <col min="10" max="10" width="28.8" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="29.19921875" customWidth="1"/>
-    <col min="14" max="14" width="19.3984375" customWidth="1"/>
+    <col min="13" max="13" width="29.2" customWidth="1"/>
+    <col min="14" max="14" width="19.4" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
+    <col min="16" max="1025" width="11.6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:14" ht="12.75" customHeight="1">
+    <row r="7" customHeight="1" spans="4:14">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +2241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="4:14" ht="12.75" customHeight="1">
+    <row r="8" customHeight="1" spans="6:14">
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1653,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:14">
+    <row r="9" spans="6:14">
       <c r="F9" t="s">
         <v>17</v>
       </c>
@@ -1682,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:14">
+    <row r="10" spans="6:14">
       <c r="F10" t="s">
         <v>20</v>
       </c>
@@ -1711,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:14">
+    <row r="11" spans="6:14">
       <c r="F11" t="s">
         <v>23</v>
       </c>
@@ -1740,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:14">
+    <row r="12" spans="6:14">
       <c r="F12" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="4:14">
+    <row r="13" spans="6:14">
       <c r="F13" t="s">
         <v>30</v>
       </c>
@@ -1798,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="4:14">
+    <row r="14" spans="6:14">
       <c r="F14" t="s">
         <v>33</v>
       </c>
@@ -1827,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="4:14">
+    <row r="15" spans="6:14">
       <c r="F15" t="s">
         <v>36</v>
       </c>
@@ -1856,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="4:14">
+    <row r="16" spans="6:14">
       <c r="F16" t="s">
         <v>39</v>
       </c>
@@ -2524,9 +3141,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -2535,32 +3151,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="D7:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F42" sqref="$A42:$XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" width="11.59765625" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" customWidth="1"/>
-    <col min="6" max="6" width="56.19921875" customWidth="1"/>
-    <col min="7" max="7" width="18.19921875" customWidth="1"/>
-    <col min="8" max="8" width="27.796875" customWidth="1"/>
+    <col min="1" max="3" width="11.6" customWidth="1"/>
+    <col min="4" max="4" width="15.2" customWidth="1"/>
+    <col min="5" max="5" width="11.6" customWidth="1"/>
+    <col min="6" max="6" width="56.2" customWidth="1"/>
+    <col min="7" max="7" width="18.2" customWidth="1"/>
+    <col min="8" max="8" width="27.8" customWidth="1"/>
     <col min="9" max="9" width="66" customWidth="1"/>
-    <col min="10" max="10" width="22.59765625" customWidth="1"/>
-    <col min="11" max="11" width="47.59765625" customWidth="1"/>
-    <col min="12" max="12" width="25.796875" customWidth="1"/>
-    <col min="13" max="13" width="37.796875" customWidth="1"/>
+    <col min="10" max="10" width="22.6" customWidth="1"/>
+    <col min="11" max="11" width="47.6" customWidth="1"/>
+    <col min="12" max="12" width="25.8" customWidth="1"/>
+    <col min="13" max="13" width="37.8" customWidth="1"/>
     <col min="14" max="14" width="27" customWidth="1"/>
-    <col min="15" max="15" width="9.796875" customWidth="1"/>
-    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
+    <col min="15" max="15" width="9.8" customWidth="1"/>
+    <col min="16" max="1025" width="11.6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:15" ht="12.75" customHeight="1">
+    <row r="7" customHeight="1" spans="4:15">
       <c r="D7" s="1" t="s">
         <v>108</v>
       </c>
@@ -2598,7 +3215,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="4:15" ht="12.75" customHeight="1">
+    <row r="8" customHeight="1" spans="6:15">
       <c r="F8" s="1" t="s">
         <v>116</v>
       </c>
@@ -2627,7 +3244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:15">
+    <row r="9" spans="6:15">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -2659,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:15">
+    <row r="10" spans="6:15">
       <c r="F10" t="s">
         <v>126</v>
       </c>
@@ -2691,7 +3308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="4:15">
+    <row r="11" spans="6:15">
       <c r="F11" t="s">
         <v>130</v>
       </c>
@@ -2723,7 +3340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="4:15">
+    <row r="12" spans="6:15">
       <c r="F12" t="s">
         <v>134</v>
       </c>
@@ -2752,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:15">
+    <row r="13" spans="6:15">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -2784,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:15">
+    <row r="14" spans="6:15">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -2816,7 +3433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:15">
+    <row r="15" spans="6:15">
       <c r="F15" t="s">
         <v>147</v>
       </c>
@@ -2848,7 +3465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="4:15">
+    <row r="16" spans="6:15">
       <c r="F16" t="s">
         <v>151</v>
       </c>
@@ -3269,7 +3886,7 @@
         <v>205</v>
       </c>
       <c r="I29" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="J29" t="s">
         <v>13</v>
@@ -3301,7 +3918,7 @@
         <v>209</v>
       </c>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J30" t="s">
         <v>13</v>
@@ -3332,6 +3949,9 @@
       <c r="H31" t="s">
         <v>213</v>
       </c>
+      <c r="I31" t="s">
+        <v>69</v>
+      </c>
       <c r="J31" t="s">
         <v>13</v>
       </c>
@@ -3342,7 +3962,7 @@
         <v>25</v>
       </c>
       <c r="M31" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="N31" t="s">
         <v>214</v>
@@ -3419,20 +4039,17 @@
       <c r="H34" t="s">
         <v>225</v>
       </c>
-      <c r="I34" t="s">
-        <v>72</v>
-      </c>
       <c r="J34" t="s">
         <v>13</v>
       </c>
       <c r="K34" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="L34" t="s">
         <v>25</v>
       </c>
       <c r="M34" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N34" t="s">
         <v>226</v>
@@ -3452,13 +4069,13 @@
         <v>229</v>
       </c>
       <c r="I35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J35" t="s">
         <v>13</v>
       </c>
       <c r="K35" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="L35" t="s">
         <v>25</v>
@@ -3484,13 +4101,13 @@
         <v>233</v>
       </c>
       <c r="I36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J36" t="s">
         <v>13</v>
       </c>
       <c r="K36" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="L36" t="s">
         <v>25</v>
@@ -3516,13 +4133,13 @@
         <v>237</v>
       </c>
       <c r="I37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J37" t="s">
         <v>13</v>
       </c>
       <c r="K37" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="L37" t="s">
         <v>25</v>
@@ -3531,7 +4148,7 @@
         <v>124</v>
       </c>
       <c r="N37" t="s">
-        <v>133</v>
+        <v>238</v>
       </c>
       <c r="O37">
         <v>12</v>
@@ -3539,16 +4156,16 @@
     </row>
     <row r="38" spans="6:15">
       <c r="F38" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G38" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H38" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J38" t="s">
         <v>13</v>
@@ -3563,7 +4180,7 @@
         <v>124</v>
       </c>
       <c r="N38" t="s">
-        <v>241</v>
+        <v>133</v>
       </c>
       <c r="O38">
         <v>13</v>
@@ -3580,13 +4197,13 @@
         <v>244</v>
       </c>
       <c r="I39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J39" t="s">
         <v>13</v>
       </c>
       <c r="K39" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L39" t="s">
         <v>25</v>
@@ -3612,13 +4229,13 @@
         <v>248</v>
       </c>
       <c r="I40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J40" t="s">
         <v>13</v>
       </c>
       <c r="K40" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="L40" t="s">
         <v>25</v>
@@ -3644,13 +4261,13 @@
         <v>252</v>
       </c>
       <c r="I41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J41" t="s">
         <v>13</v>
       </c>
       <c r="K41" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="L41" t="s">
         <v>25</v>
@@ -3676,13 +4293,13 @@
         <v>256</v>
       </c>
       <c r="I42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J42" t="s">
         <v>13</v>
       </c>
       <c r="K42" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="L42" t="s">
         <v>25</v>
@@ -3852,9 +4469,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -3863,24 +4479,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="D7:G161"/>
   <sheetViews>
-    <sheetView topLeftCell="D133" workbookViewId="0">
+    <sheetView topLeftCell="D112" workbookViewId="0">
       <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="3" width="11.59765625" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="1" max="3" width="11.6" customWidth="1"/>
+    <col min="4" max="4" width="23.8" customWidth="1"/>
+    <col min="5" max="5" width="11.6" customWidth="1"/>
     <col min="6" max="6" width="82" customWidth="1"/>
-    <col min="7" max="7" width="85.19921875" customWidth="1"/>
-    <col min="8" max="1025" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="85.2" customWidth="1"/>
+    <col min="8" max="1025" width="11.6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="12.75" customHeight="1">
+    <row r="7" customHeight="1" spans="4:7">
       <c r="D7" s="1" t="s">
         <v>278</v>
       </c>
@@ -3894,7 +4511,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="4:7" ht="12.75" customHeight="1">
+    <row r="8" customHeight="1" spans="6:7">
       <c r="F8" t="s">
         <v>121</v>
       </c>
@@ -3902,7 +4519,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="4:7">
+    <row r="9" spans="6:7">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -3910,7 +4527,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="4:7">
+    <row r="10" spans="6:7">
       <c r="F10" t="s">
         <v>121</v>
       </c>
@@ -3918,7 +4535,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="4:7">
+    <row r="11" spans="6:7">
       <c r="F11" t="s">
         <v>126</v>
       </c>
@@ -3926,7 +4543,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="4:7">
+    <row r="12" spans="6:7">
       <c r="F12" t="s">
         <v>130</v>
       </c>
@@ -3934,7 +4551,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="4:7">
+    <row r="13" spans="6:7">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -3942,7 +4559,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="4:7">
+    <row r="14" spans="6:7">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -3950,7 +4567,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="4:7">
+    <row r="15" spans="6:7">
       <c r="F15" t="s">
         <v>143</v>
       </c>
@@ -3958,7 +4575,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="4:7">
+    <row r="16" spans="6:7">
       <c r="F16" t="s">
         <v>147</v>
       </c>
@@ -4448,7 +5065,7 @@
     </row>
     <row r="77" spans="6:7">
       <c r="F77" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G77" t="s">
         <v>317</v>
@@ -4456,7 +5073,7 @@
     </row>
     <row r="78" spans="6:7">
       <c r="F78" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G78" t="s">
         <v>314</v>
@@ -4464,7 +5081,7 @@
     </row>
     <row r="79" spans="6:7">
       <c r="F79" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G79" t="s">
         <v>315</v>
@@ -4472,7 +5089,7 @@
     </row>
     <row r="80" spans="6:7">
       <c r="F80" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G80" t="s">
         <v>316</v>
@@ -4480,7 +5097,7 @@
     </row>
     <row r="81" spans="6:7">
       <c r="F81" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G81" t="s">
         <v>317</v>
@@ -4488,7 +5105,7 @@
     </row>
     <row r="82" spans="6:7">
       <c r="F82" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G82" t="s">
         <v>318</v>
@@ -4496,7 +5113,7 @@
     </row>
     <row r="83" spans="6:7">
       <c r="F83" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G83" t="s">
         <v>319</v>
@@ -4504,7 +5121,7 @@
     </row>
     <row r="84" spans="6:7">
       <c r="F84" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G84" t="s">
         <v>320</v>
@@ -4512,7 +5129,7 @@
     </row>
     <row r="85" spans="6:7">
       <c r="F85" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G85" t="s">
         <v>321</v>
@@ -4520,7 +5137,7 @@
     </row>
     <row r="86" spans="6:7">
       <c r="F86" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G86" t="s">
         <v>322</v>
@@ -4528,7 +5145,7 @@
     </row>
     <row r="87" spans="6:7">
       <c r="F87" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G87" t="s">
         <v>323</v>
@@ -4536,7 +5153,7 @@
     </row>
     <row r="88" spans="6:7">
       <c r="F88" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G88" t="s">
         <v>324</v>
@@ -4544,7 +5161,7 @@
     </row>
     <row r="89" spans="6:7">
       <c r="F89" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G89" t="s">
         <v>325</v>
@@ -4552,7 +5169,7 @@
     </row>
     <row r="90" spans="6:7">
       <c r="F90" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G90" t="s">
         <v>326</v>
@@ -4560,7 +5177,7 @@
     </row>
     <row r="91" spans="6:7">
       <c r="F91" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G91" t="s">
         <v>329</v>
@@ -4568,7 +5185,7 @@
     </row>
     <row r="92" spans="6:7">
       <c r="F92" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G92" t="s">
         <v>330</v>
@@ -4576,7 +5193,7 @@
     </row>
     <row r="93" spans="6:7">
       <c r="F93" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G93" t="s">
         <v>331</v>
@@ -4584,7 +5201,7 @@
     </row>
     <row r="94" spans="6:7">
       <c r="F94" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G94" t="s">
         <v>332</v>
@@ -4592,7 +5209,7 @@
     </row>
     <row r="95" spans="6:7">
       <c r="F95" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G95" t="s">
         <v>336</v>
@@ -4600,7 +5217,7 @@
     </row>
     <row r="96" spans="6:7">
       <c r="F96" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G96" t="s">
         <v>333</v>
@@ -4608,7 +5225,7 @@
     </row>
     <row r="97" spans="6:7">
       <c r="F97" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G97" t="s">
         <v>334</v>
@@ -4616,7 +5233,7 @@
     </row>
     <row r="98" spans="6:7">
       <c r="F98" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G98" t="s">
         <v>335</v>
@@ -4624,7 +5241,7 @@
     </row>
     <row r="99" spans="6:7">
       <c r="F99" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G99" t="s">
         <v>339</v>
@@ -4632,7 +5249,7 @@
     </row>
     <row r="100" spans="6:7">
       <c r="F100" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G100" t="s">
         <v>337</v>
@@ -4640,7 +5257,7 @@
     </row>
     <row r="101" spans="6:7">
       <c r="F101" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G101" t="s">
         <v>338</v>
@@ -4648,7 +5265,7 @@
     </row>
     <row r="102" spans="6:7">
       <c r="F102" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G102" t="s">
         <v>342</v>
@@ -4656,7 +5273,7 @@
     </row>
     <row r="103" spans="6:7">
       <c r="F103" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G103" t="s">
         <v>343</v>
@@ -4664,7 +5281,7 @@
     </row>
     <row r="104" spans="6:7">
       <c r="F104" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G104" t="s">
         <v>344</v>
@@ -4672,7 +5289,7 @@
     </row>
     <row r="105" spans="6:7">
       <c r="F105" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G105" t="s">
         <v>345</v>
@@ -4680,7 +5297,7 @@
     </row>
     <row r="106" spans="6:7">
       <c r="F106" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G106" t="s">
         <v>329</v>
@@ -4688,7 +5305,7 @@
     </row>
     <row r="107" spans="6:7">
       <c r="F107" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G107" t="s">
         <v>346</v>
@@ -4696,7 +5313,7 @@
     </row>
     <row r="108" spans="6:7">
       <c r="F108" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G108" t="s">
         <v>347</v>
@@ -4704,7 +5321,7 @@
     </row>
     <row r="109" spans="6:7">
       <c r="F109" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="G109" t="s">
         <v>348</v>
@@ -4712,7 +5329,7 @@
     </row>
     <row r="110" spans="6:7">
       <c r="F110" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G110" t="s">
         <v>349</v>
@@ -4720,7 +5337,7 @@
     </row>
     <row r="111" spans="6:7">
       <c r="F111" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G111" t="s">
         <v>350</v>
@@ -4728,7 +5345,7 @@
     </row>
     <row r="112" spans="6:7">
       <c r="F112" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G112" t="s">
         <v>351</v>
@@ -4736,7 +5353,7 @@
     </row>
     <row r="113" spans="6:7">
       <c r="F113" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="G113" t="s">
         <v>352</v>
@@ -4744,7 +5361,7 @@
     </row>
     <row r="114" spans="6:7">
       <c r="F114" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G114" t="s">
         <v>353</v>
@@ -4752,7 +5369,7 @@
     </row>
     <row r="115" spans="6:7">
       <c r="F115" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G115" t="s">
         <v>354</v>
@@ -4760,7 +5377,7 @@
     </row>
     <row r="116" spans="6:7">
       <c r="F116" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G116" t="s">
         <v>355</v>
@@ -4768,7 +5385,7 @@
     </row>
     <row r="117" spans="6:7">
       <c r="F117" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G117" t="s">
         <v>356</v>
@@ -4776,7 +5393,7 @@
     </row>
     <row r="118" spans="6:7">
       <c r="F118" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G118" t="s">
         <v>357</v>
@@ -4784,7 +5401,7 @@
     </row>
     <row r="119" spans="6:7">
       <c r="F119" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G119" t="s">
         <v>358</v>
@@ -4792,7 +5409,7 @@
     </row>
     <row r="120" spans="6:7">
       <c r="F120" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G120" t="s">
         <v>359</v>
@@ -4800,7 +5417,7 @@
     </row>
     <row r="121" spans="6:7">
       <c r="F121" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G121" t="s">
         <v>360</v>
@@ -4808,7 +5425,7 @@
     </row>
     <row r="122" spans="6:7">
       <c r="F122" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G122" t="s">
         <v>361</v>
@@ -4816,7 +5433,7 @@
     </row>
     <row r="123" spans="6:7">
       <c r="F123" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G123" t="s">
         <v>362</v>
@@ -4824,7 +5441,7 @@
     </row>
     <row r="124" spans="6:7">
       <c r="F124" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G124" t="s">
         <v>363</v>
@@ -4832,7 +5449,7 @@
     </row>
     <row r="125" spans="6:7">
       <c r="F125" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G125" t="s">
         <v>364</v>
@@ -4840,7 +5457,7 @@
     </row>
     <row r="126" spans="6:7">
       <c r="F126" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G126" t="s">
         <v>363</v>
@@ -4848,7 +5465,7 @@
     </row>
     <row r="127" spans="6:7">
       <c r="F127" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G127" t="s">
         <v>365</v>
@@ -4856,7 +5473,7 @@
     </row>
     <row r="128" spans="6:7">
       <c r="F128" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G128" t="s">
         <v>366</v>
@@ -4864,7 +5481,7 @@
     </row>
     <row r="129" spans="6:7">
       <c r="F129" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G129" t="s">
         <v>367</v>
@@ -4872,7 +5489,7 @@
     </row>
     <row r="130" spans="6:7">
       <c r="F130" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G130" t="s">
         <v>368</v>
@@ -4880,7 +5497,7 @@
     </row>
     <row r="131" spans="6:7">
       <c r="F131" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="G131" t="s">
         <v>369</v>
@@ -4888,7 +5505,7 @@
     </row>
     <row r="132" spans="6:7">
       <c r="F132" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="G132" t="s">
         <v>370</v>
@@ -4896,7 +5513,7 @@
     </row>
     <row r="133" spans="6:7">
       <c r="F133" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="G133" t="s">
         <v>371</v>
@@ -4904,7 +5521,7 @@
     </row>
     <row r="134" spans="6:7">
       <c r="F134" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="G134" t="s">
         <v>372</v>
@@ -5127,9 +5744,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[ADD]the menu file add FD_CATEGORY_MENU sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyongle/Documents/work/service/devops-service/src/main/resources/script/front/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D6D01B-3960-744A-A4EB-C0DB4C36DD43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19935" windowHeight="7785" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
     <sheet name="IAM_MENU_B" sheetId="2" r:id="rId2"/>
-    <sheet name="IAM_MENU_PERMISSION" sheetId="3" r:id="rId3"/>
+    <sheet name="FD_CATEGORY_MENU" sheetId="4" r:id="rId3"/>
+    <sheet name="IAM_MENU_PERMISSION" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="404">
   <si>
     <t>IAM_PERMISSION</t>
   </si>
@@ -1204,19 +1211,45 @@
   </si>
   <si>
     <t>devops-service.devops-gitlab-pipeline.listPipelineFrequency</t>
+  </si>
+  <si>
+    <t>FD_CATEGORY_MENU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>*ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>#CATEGORY_CODE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>#MENU_CODE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>#RESOURCE_LEVEL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGILE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>organization_project</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Droid Sans Fallback"/>
@@ -1230,355 +1263,24 @@
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1586,312 +1288,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2176,37 +1592,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D7:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="131" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="11.6" customWidth="1"/>
-    <col min="6" max="6" width="65.8" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="6" max="6" width="65.796875" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="28.8" customWidth="1"/>
+    <col min="10" max="10" width="28.796875" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="29.2" customWidth="1"/>
-    <col min="14" max="14" width="19.4" customWidth="1"/>
+    <col min="13" max="13" width="29.19921875" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="1025" width="11.6" customWidth="1"/>
+    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" customHeight="1" spans="4:14">
+    <row r="7" spans="4:14" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2241,7 +1657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="6:14">
+    <row r="8" spans="4:14" ht="12.75" customHeight="1">
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="6:14">
+    <row r="9" spans="4:14">
       <c r="F9" t="s">
         <v>17</v>
       </c>
@@ -2299,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="6:14">
+    <row r="10" spans="4:14">
       <c r="F10" t="s">
         <v>20</v>
       </c>
@@ -2328,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="6:14">
+    <row r="11" spans="4:14">
       <c r="F11" t="s">
         <v>23</v>
       </c>
@@ -2357,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="6:14">
+    <row r="12" spans="4:14">
       <c r="F12" t="s">
         <v>27</v>
       </c>
@@ -2386,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="6:14">
+    <row r="13" spans="4:14">
       <c r="F13" t="s">
         <v>30</v>
       </c>
@@ -2415,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="6:14">
+    <row r="14" spans="4:14">
       <c r="F14" t="s">
         <v>33</v>
       </c>
@@ -2444,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="6:14">
+    <row r="15" spans="4:14">
       <c r="F15" t="s">
         <v>36</v>
       </c>
@@ -2473,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="6:14">
+    <row r="16" spans="4:14">
       <c r="F16" t="s">
         <v>39</v>
       </c>
@@ -3141,8 +2557,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -3151,33 +2568,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D7:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F42" sqref="$A42:$XFD42"/>
+    <sheetView topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6" customWidth="1"/>
-    <col min="4" max="4" width="15.2" customWidth="1"/>
-    <col min="5" max="5" width="11.6" customWidth="1"/>
-    <col min="6" max="6" width="56.2" customWidth="1"/>
-    <col min="7" max="7" width="18.2" customWidth="1"/>
-    <col min="8" max="8" width="27.8" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="6" max="6" width="56.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.19921875" customWidth="1"/>
+    <col min="8" max="8" width="27.796875" customWidth="1"/>
     <col min="9" max="9" width="66" customWidth="1"/>
-    <col min="10" max="10" width="22.6" customWidth="1"/>
-    <col min="11" max="11" width="47.6" customWidth="1"/>
-    <col min="12" max="12" width="25.8" customWidth="1"/>
-    <col min="13" max="13" width="37.8" customWidth="1"/>
+    <col min="10" max="10" width="22.59765625" customWidth="1"/>
+    <col min="11" max="11" width="47.59765625" customWidth="1"/>
+    <col min="12" max="12" width="25.796875" customWidth="1"/>
+    <col min="13" max="13" width="37.796875" customWidth="1"/>
     <col min="14" max="14" width="27" customWidth="1"/>
-    <col min="15" max="15" width="9.8" customWidth="1"/>
-    <col min="16" max="1025" width="11.6" customWidth="1"/>
+    <col min="15" max="15" width="9.796875" customWidth="1"/>
+    <col min="16" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" customHeight="1" spans="4:15">
+    <row r="7" spans="4:15" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>108</v>
       </c>
@@ -3215,7 +2631,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="6:15">
+    <row r="8" spans="4:15" ht="12.75" customHeight="1">
       <c r="F8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3244,7 +2660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="6:15">
+    <row r="9" spans="4:15">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -3276,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="6:15">
+    <row r="10" spans="4:15">
       <c r="F10" t="s">
         <v>126</v>
       </c>
@@ -3308,7 +2724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="6:15">
+    <row r="11" spans="4:15">
       <c r="F11" t="s">
         <v>130</v>
       </c>
@@ -3340,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="6:15">
+    <row r="12" spans="4:15">
       <c r="F12" t="s">
         <v>134</v>
       </c>
@@ -3369,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="6:15">
+    <row r="13" spans="4:15">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -3401,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="6:15">
+    <row r="14" spans="4:15">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -3433,7 +2849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="6:15">
+    <row r="15" spans="4:15">
       <c r="F15" t="s">
         <v>147</v>
       </c>
@@ -3465,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="6:15">
+    <row r="16" spans="4:15">
       <c r="F16" t="s">
         <v>151</v>
       </c>
@@ -4469,8 +3885,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>
@@ -4479,25 +3896,899 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786B14DF-DF88-B34D-A0E3-421049572596}">
+  <dimension ref="D7:H83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="54.796875" customWidth="1"/>
+    <col min="8" max="8" width="28.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:8">
+      <c r="D7" t="s">
+        <v>396</v>
+      </c>
+      <c r="E7" t="s">
+        <v>397</v>
+      </c>
+      <c r="F7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G7" t="s">
+        <v>399</v>
+      </c>
+      <c r="H7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8">
+      <c r="F8" t="s">
+        <v>401</v>
+      </c>
+      <c r="G8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8">
+      <c r="F9" t="s">
+        <v>401</v>
+      </c>
+      <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8">
+      <c r="F10" t="s">
+        <v>401</v>
+      </c>
+      <c r="G10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8">
+      <c r="F11" t="s">
+        <v>401</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8">
+      <c r="F12" t="s">
+        <v>401</v>
+      </c>
+      <c r="G12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8">
+      <c r="F13" t="s">
+        <v>401</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8">
+      <c r="F14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8">
+      <c r="F15" t="s">
+        <v>401</v>
+      </c>
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8">
+      <c r="F16" t="s">
+        <v>401</v>
+      </c>
+      <c r="G16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8">
+      <c r="F17" t="s">
+        <v>401</v>
+      </c>
+      <c r="G17" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8">
+      <c r="F18" t="s">
+        <v>401</v>
+      </c>
+      <c r="G18" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8">
+      <c r="F19" t="s">
+        <v>401</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8">
+      <c r="F20" t="s">
+        <v>401</v>
+      </c>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8">
+      <c r="F21" t="s">
+        <v>401</v>
+      </c>
+      <c r="G21" t="s">
+        <v>171</v>
+      </c>
+      <c r="H21" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8">
+      <c r="F22" t="s">
+        <v>401</v>
+      </c>
+      <c r="G22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8">
+      <c r="F23" t="s">
+        <v>401</v>
+      </c>
+      <c r="G23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="6:8">
+      <c r="F24" t="s">
+        <v>401</v>
+      </c>
+      <c r="G24" t="s">
+        <v>183</v>
+      </c>
+      <c r="H24" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="6:8">
+      <c r="F25" t="s">
+        <v>401</v>
+      </c>
+      <c r="G25" t="s">
+        <v>187</v>
+      </c>
+      <c r="H25" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8">
+      <c r="F26" t="s">
+        <v>401</v>
+      </c>
+      <c r="G26" t="s">
+        <v>191</v>
+      </c>
+      <c r="H26" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="6:8">
+      <c r="F27" t="s">
+        <v>401</v>
+      </c>
+      <c r="G27" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8">
+      <c r="F28" t="s">
+        <v>401</v>
+      </c>
+      <c r="G28" t="s">
+        <v>199</v>
+      </c>
+      <c r="H28" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="29" spans="6:8">
+      <c r="F29" t="s">
+        <v>401</v>
+      </c>
+      <c r="G29" t="s">
+        <v>203</v>
+      </c>
+      <c r="H29" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8">
+      <c r="F30" t="s">
+        <v>401</v>
+      </c>
+      <c r="G30" t="s">
+        <v>207</v>
+      </c>
+      <c r="H30" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="31" spans="6:8">
+      <c r="F31" t="s">
+        <v>401</v>
+      </c>
+      <c r="G31" t="s">
+        <v>211</v>
+      </c>
+      <c r="H31" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="6:8">
+      <c r="F32" t="s">
+        <v>401</v>
+      </c>
+      <c r="G32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8">
+      <c r="F33" t="s">
+        <v>401</v>
+      </c>
+      <c r="G33" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8">
+      <c r="F34" t="s">
+        <v>401</v>
+      </c>
+      <c r="G34" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8">
+      <c r="F35" t="s">
+        <v>401</v>
+      </c>
+      <c r="G35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H35" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8">
+      <c r="F36" t="s">
+        <v>401</v>
+      </c>
+      <c r="G36" t="s">
+        <v>231</v>
+      </c>
+      <c r="H36" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8">
+      <c r="F37" t="s">
+        <v>401</v>
+      </c>
+      <c r="G37" t="s">
+        <v>235</v>
+      </c>
+      <c r="H37" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8">
+      <c r="F38" t="s">
+        <v>401</v>
+      </c>
+      <c r="G38" t="s">
+        <v>239</v>
+      </c>
+      <c r="H38" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8">
+      <c r="F39" t="s">
+        <v>401</v>
+      </c>
+      <c r="G39" t="s">
+        <v>242</v>
+      </c>
+      <c r="H39" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8">
+      <c r="F40" t="s">
+        <v>401</v>
+      </c>
+      <c r="G40" t="s">
+        <v>246</v>
+      </c>
+      <c r="H40" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8">
+      <c r="F41" t="s">
+        <v>401</v>
+      </c>
+      <c r="G41" t="s">
+        <v>250</v>
+      </c>
+      <c r="H41" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8">
+      <c r="F42" t="s">
+        <v>401</v>
+      </c>
+      <c r="G42" t="s">
+        <v>254</v>
+      </c>
+      <c r="H42" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8">
+      <c r="F43" t="s">
+        <v>401</v>
+      </c>
+      <c r="G43" t="s">
+        <v>258</v>
+      </c>
+      <c r="H43" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8">
+      <c r="F44" t="s">
+        <v>401</v>
+      </c>
+      <c r="G44" t="s">
+        <v>262</v>
+      </c>
+      <c r="H44" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8">
+      <c r="F45" t="s">
+        <v>401</v>
+      </c>
+      <c r="G45" t="s">
+        <v>266</v>
+      </c>
+      <c r="H45" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8">
+      <c r="F46" t="s">
+        <v>401</v>
+      </c>
+      <c r="G46" t="s">
+        <v>270</v>
+      </c>
+      <c r="H46" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8">
+      <c r="F47" t="s">
+        <v>401</v>
+      </c>
+      <c r="G47" t="s">
+        <v>274</v>
+      </c>
+      <c r="H47" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8">
+      <c r="F48" t="s">
+        <v>402</v>
+      </c>
+      <c r="G48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8">
+      <c r="F49" t="s">
+        <v>402</v>
+      </c>
+      <c r="G49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8">
+      <c r="F50" t="s">
+        <v>402</v>
+      </c>
+      <c r="G50" t="s">
+        <v>143</v>
+      </c>
+      <c r="H50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8">
+      <c r="F51" t="s">
+        <v>402</v>
+      </c>
+      <c r="G51" t="s">
+        <v>147</v>
+      </c>
+      <c r="H51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8">
+      <c r="F52" t="s">
+        <v>402</v>
+      </c>
+      <c r="G52" t="s">
+        <v>151</v>
+      </c>
+      <c r="H52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8">
+      <c r="F53" t="s">
+        <v>402</v>
+      </c>
+      <c r="G53" t="s">
+        <v>155</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8">
+      <c r="F54" t="s">
+        <v>402</v>
+      </c>
+      <c r="G54" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8">
+      <c r="F55" t="s">
+        <v>402</v>
+      </c>
+      <c r="G55" t="s">
+        <v>163</v>
+      </c>
+      <c r="H55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8">
+      <c r="F56" t="s">
+        <v>402</v>
+      </c>
+      <c r="G56" t="s">
+        <v>167</v>
+      </c>
+      <c r="H56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8">
+      <c r="F57" t="s">
+        <v>402</v>
+      </c>
+      <c r="G57" t="s">
+        <v>171</v>
+      </c>
+      <c r="H57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8">
+      <c r="F58" t="s">
+        <v>402</v>
+      </c>
+      <c r="G58" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8">
+      <c r="F59" t="s">
+        <v>402</v>
+      </c>
+      <c r="G59" t="s">
+        <v>179</v>
+      </c>
+      <c r="H59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8">
+      <c r="F60" t="s">
+        <v>402</v>
+      </c>
+      <c r="G60" t="s">
+        <v>183</v>
+      </c>
+      <c r="H60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8">
+      <c r="F61" t="s">
+        <v>402</v>
+      </c>
+      <c r="G61" t="s">
+        <v>187</v>
+      </c>
+      <c r="H61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8">
+      <c r="F62" t="s">
+        <v>402</v>
+      </c>
+      <c r="G62" t="s">
+        <v>191</v>
+      </c>
+      <c r="H62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8">
+      <c r="F63" t="s">
+        <v>402</v>
+      </c>
+      <c r="G63" t="s">
+        <v>195</v>
+      </c>
+      <c r="H63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8">
+      <c r="F64" t="s">
+        <v>402</v>
+      </c>
+      <c r="G64" t="s">
+        <v>199</v>
+      </c>
+      <c r="H64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8">
+      <c r="F65" t="s">
+        <v>402</v>
+      </c>
+      <c r="G65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8">
+      <c r="F66" t="s">
+        <v>402</v>
+      </c>
+      <c r="G66" t="s">
+        <v>207</v>
+      </c>
+      <c r="H66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8">
+      <c r="F67" t="s">
+        <v>402</v>
+      </c>
+      <c r="G67" t="s">
+        <v>211</v>
+      </c>
+      <c r="H67" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8">
+      <c r="F68" t="s">
+        <v>402</v>
+      </c>
+      <c r="G68" t="s">
+        <v>215</v>
+      </c>
+      <c r="H68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8">
+      <c r="F69" t="s">
+        <v>402</v>
+      </c>
+      <c r="G69" t="s">
+        <v>219</v>
+      </c>
+      <c r="H69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8">
+      <c r="F70" t="s">
+        <v>402</v>
+      </c>
+      <c r="G70" t="s">
+        <v>223</v>
+      </c>
+      <c r="H70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8">
+      <c r="F71" t="s">
+        <v>402</v>
+      </c>
+      <c r="G71" t="s">
+        <v>227</v>
+      </c>
+      <c r="H71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8">
+      <c r="F72" t="s">
+        <v>402</v>
+      </c>
+      <c r="G72" t="s">
+        <v>231</v>
+      </c>
+      <c r="H72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8">
+      <c r="F73" t="s">
+        <v>402</v>
+      </c>
+      <c r="G73" t="s">
+        <v>235</v>
+      </c>
+      <c r="H73" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8">
+      <c r="F74" t="s">
+        <v>402</v>
+      </c>
+      <c r="G74" t="s">
+        <v>239</v>
+      </c>
+      <c r="H74" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8">
+      <c r="F75" t="s">
+        <v>402</v>
+      </c>
+      <c r="G75" t="s">
+        <v>242</v>
+      </c>
+      <c r="H75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8">
+      <c r="F76" t="s">
+        <v>402</v>
+      </c>
+      <c r="G76" t="s">
+        <v>246</v>
+      </c>
+      <c r="H76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8">
+      <c r="F77" t="s">
+        <v>402</v>
+      </c>
+      <c r="G77" t="s">
+        <v>250</v>
+      </c>
+      <c r="H77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8">
+      <c r="F78" t="s">
+        <v>402</v>
+      </c>
+      <c r="G78" t="s">
+        <v>254</v>
+      </c>
+      <c r="H78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8">
+      <c r="F79" t="s">
+        <v>402</v>
+      </c>
+      <c r="G79" t="s">
+        <v>258</v>
+      </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8">
+      <c r="F80" t="s">
+        <v>402</v>
+      </c>
+      <c r="G80" t="s">
+        <v>262</v>
+      </c>
+      <c r="H80" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8">
+      <c r="F81" t="s">
+        <v>402</v>
+      </c>
+      <c r="G81" t="s">
+        <v>266</v>
+      </c>
+      <c r="H81" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8">
+      <c r="F82" t="s">
+        <v>402</v>
+      </c>
+      <c r="G82" t="s">
+        <v>270</v>
+      </c>
+      <c r="H82" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8">
+      <c r="F83" t="s">
+        <v>402</v>
+      </c>
+      <c r="G83" t="s">
+        <v>274</v>
+      </c>
+      <c r="H83" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D7:G161"/>
   <sheetViews>
     <sheetView topLeftCell="D112" workbookViewId="0">
       <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="3" width="11.6" customWidth="1"/>
-    <col min="4" max="4" width="23.8" customWidth="1"/>
-    <col min="5" max="5" width="11.6" customWidth="1"/>
+    <col min="1" max="3" width="11.59765625" customWidth="1"/>
+    <col min="4" max="4" width="23.796875" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
     <col min="6" max="6" width="82" customWidth="1"/>
-    <col min="7" max="7" width="85.2" customWidth="1"/>
-    <col min="8" max="1025" width="11.6" customWidth="1"/>
+    <col min="7" max="7" width="85.19921875" customWidth="1"/>
+    <col min="8" max="1025" width="11.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" customHeight="1" spans="4:7">
+    <row r="7" spans="4:7" ht="12.75" customHeight="1">
       <c r="D7" s="1" t="s">
         <v>278</v>
       </c>
@@ -4511,7 +4802,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="6:7">
+    <row r="8" spans="4:7" ht="12.75" customHeight="1">
       <c r="F8" t="s">
         <v>121</v>
       </c>
@@ -4519,7 +4810,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="6:7">
+    <row r="9" spans="4:7">
       <c r="F9" t="s">
         <v>121</v>
       </c>
@@ -4527,7 +4818,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="6:7">
+    <row r="10" spans="4:7">
       <c r="F10" t="s">
         <v>121</v>
       </c>
@@ -4535,7 +4826,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="6:7">
+    <row r="11" spans="4:7">
       <c r="F11" t="s">
         <v>126</v>
       </c>
@@ -4543,7 +4834,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="6:7">
+    <row r="12" spans="4:7">
       <c r="F12" t="s">
         <v>130</v>
       </c>
@@ -4551,7 +4842,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="6:7">
+    <row r="13" spans="4:7">
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -4559,7 +4850,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="6:7">
+    <row r="14" spans="4:7">
       <c r="F14" t="s">
         <v>143</v>
       </c>
@@ -4567,7 +4858,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="6:7">
+    <row r="15" spans="4:7">
       <c r="F15" t="s">
         <v>143</v>
       </c>
@@ -4575,7 +4866,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="6:7">
+    <row r="16" spans="4:7">
       <c r="F16" t="s">
         <v>147</v>
       </c>
@@ -5744,8 +6035,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12 Page &amp;P</oddFooter>

</xml_diff>